<commit_message>
Provide on GitHub for Presentation
</commit_message>
<xml_diff>
--- a/In Class Demo - NCT03417583.xlsx
+++ b/In Class Demo - NCT03417583.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="25360" windowHeight="16500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="28560" windowHeight="16500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Criteria2Query" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="192">
   <si>
     <t>Recognized Text</t>
   </si>
@@ -230,14 +230,388 @@
   </si>
   <si>
     <t>Concept Name</t>
+  </si>
+  <si>
+    <t>C0030705</t>
+  </si>
+  <si>
+    <t>UMLS Entity</t>
+  </si>
+  <si>
+    <t>UMLS Domain</t>
+  </si>
+  <si>
+    <t>UMLS CUI</t>
+  </si>
+  <si>
+    <t>UMLS Source(s)</t>
+  </si>
+  <si>
+    <t>Patient (Patients)</t>
+  </si>
+  <si>
+    <t>LNC,LNC,SNOMEDCT_US,SNOMEDCT_US,SNOMEDCT_US</t>
+  </si>
+  <si>
+    <t>UPDRS (Unified Parkinson's Disease Rating Scale)</t>
+  </si>
+  <si>
+    <t>C3639721</t>
+  </si>
+  <si>
+    <t>LNC, LNC</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Patient or Disabled Group</t>
+  </si>
+  <si>
+    <t>Intellectual Product</t>
+  </si>
+  <si>
+    <t>Quantitative Concept</t>
+  </si>
+  <si>
+    <t>C0449820</t>
+  </si>
+  <si>
+    <t>Drugs (Pharmaceutical Preparations)</t>
+  </si>
+  <si>
+    <t>Pharmacologic Substance</t>
+  </si>
+  <si>
+    <t>C0013227</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>C0205250</t>
+  </si>
+  <si>
+    <t>Qualitative Concept</t>
+  </si>
+  <si>
+    <t>Mild to moderate</t>
+  </si>
+  <si>
+    <t>C1299392</t>
+  </si>
+  <si>
+    <t>C0441766</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Stage Level 1</t>
+  </si>
+  <si>
+    <t>&lt; 3 (qualifier value)</t>
+  </si>
+  <si>
+    <t>C0439086</t>
+  </si>
+  <si>
+    <t>SNOMEDCT_US,SNOMEDCT_US,SNOMEDCT_US</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Age Group</t>
+  </si>
+  <si>
+    <t>C0001675</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>partially_correct</t>
+  </si>
+  <si>
+    <t>incorrect</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>C0439234</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Temporal Concept</t>
+  </si>
+  <si>
+    <t>Old age</t>
+  </si>
+  <si>
+    <t>Population Group</t>
+  </si>
+  <si>
+    <t>C1999167</t>
+  </si>
+  <si>
+    <t>Woman</t>
+  </si>
+  <si>
+    <t>C0043210</t>
+  </si>
+  <si>
+    <t>Gravida NOS (Gravidity)</t>
+  </si>
+  <si>
+    <t>Finding</t>
+  </si>
+  <si>
+    <t>C0600457</t>
+  </si>
+  <si>
+    <t>Nursing care, NOS (nursing therapy)</t>
+  </si>
+  <si>
+    <t>Therapeutic or Preventive Procedure</t>
+  </si>
+  <si>
+    <t>C0028678</t>
+  </si>
+  <si>
+    <t>H/O: cardiovascular disease</t>
+  </si>
+  <si>
+    <t>C0455539</t>
+  </si>
+  <si>
+    <t>Significant</t>
+  </si>
+  <si>
+    <t>Idea or Concept</t>
+  </si>
+  <si>
+    <t>C0750502</t>
+  </si>
+  <si>
+    <t>Artificial cardiac pacemaker</t>
+  </si>
+  <si>
+    <t>Medical Device</t>
+  </si>
+  <si>
+    <t>C0030163</t>
+  </si>
+  <si>
+    <t>History of mood disorder</t>
+  </si>
+  <si>
+    <t>C1996950</t>
+  </si>
+  <si>
+    <t>C0443343</t>
+  </si>
+  <si>
+    <t>Unstable status</t>
+  </si>
+  <si>
+    <t>Anxiety disorder (Anxiety Disorders)</t>
+  </si>
+  <si>
+    <t>Mental or Behavioral Dysfunction</t>
+  </si>
+  <si>
+    <t>C0003469</t>
+  </si>
+  <si>
+    <t>ICD10CM,LNC,LNC,SNOMEDCT_US,SNOMEDCT_US,SNOMEDCT_US</t>
+  </si>
+  <si>
+    <t>Psychotic disorder (Psychotic Disorders)</t>
+  </si>
+  <si>
+    <t>ICD9CM,ICD9CM,LNC,LNC,SNOMEDCT_US,SNOMEDCT_US,SNOMEDCT_US</t>
+  </si>
+  <si>
+    <t>C0033975</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Functional Concept</t>
+  </si>
+  <si>
+    <t>C0457083</t>
+  </si>
+  <si>
+    <t>Hearing aid (Hearing Aids)</t>
+  </si>
+  <si>
+    <t>C0018768</t>
+  </si>
+  <si>
+    <t>Implantation of cochlear prosthetic device (Cochlear implant procedure)</t>
+  </si>
+  <si>
+    <t>C0302559</t>
+  </si>
+  <si>
+    <t>C0011900</t>
+  </si>
+  <si>
+    <t>Diagnostic Procedure</t>
+  </si>
+  <si>
+    <t>Diagnosis</t>
+  </si>
+  <si>
+    <t>Nervous system disorders NOS (nervous system disorder)</t>
+  </si>
+  <si>
+    <t>ICD10CM,ICD9CM,ICD9CM,LNC,LNC,SNOMEDCT_US,SNOMEDCT_US,SNOMEDCT_US</t>
+  </si>
+  <si>
+    <t>C0027765</t>
+  </si>
+  <si>
+    <t>Disease or Syndrome</t>
+  </si>
+  <si>
+    <t>C0012634</t>
+  </si>
+  <si>
+    <t>Disease</t>
+  </si>
+  <si>
+    <t>Atypical parkinsonism</t>
+  </si>
+  <si>
+    <t>C4302185</t>
+  </si>
+  <si>
+    <t>C1735318</t>
+  </si>
+  <si>
+    <t>Vestibular apparatus (Vestibular Labyrinth)</t>
+  </si>
+  <si>
+    <t>Body Part, Organ, or Organ Component</t>
+  </si>
+  <si>
+    <t>Functional disorder</t>
+  </si>
+  <si>
+    <t>C0277785</t>
+  </si>
+  <si>
+    <t>Pathologic Function</t>
+  </si>
+  <si>
+    <t>C0086190</t>
+  </si>
+  <si>
+    <t>Hazardous or Poisonous Substance</t>
+  </si>
+  <si>
+    <t>Drugs of abuse (Illicit Drugs)</t>
+  </si>
+  <si>
+    <t>Organic Chemical,Pharmacologic Substance</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>C0001962</t>
+  </si>
+  <si>
+    <t>Eye surgery (Ophthalmic surgery specialty)</t>
+  </si>
+  <si>
+    <t>Biomedical Occupation or Discipline</t>
+  </si>
+  <si>
+    <t>C1705869</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>C0205156</t>
+  </si>
+  <si>
+    <t>Three months</t>
+  </si>
+  <si>
+    <t>C4082119</t>
+  </si>
+  <si>
+    <t>Entire ear</t>
+  </si>
+  <si>
+    <t>C0521421</t>
+  </si>
+  <si>
+    <t>Six months</t>
+  </si>
+  <si>
+    <t>C4082120</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>C0205177</t>
+  </si>
+  <si>
+    <t>C0699744</t>
+  </si>
+  <si>
+    <t>Clinical trial (Clinical Trials)</t>
+  </si>
+  <si>
+    <t>Research Activity</t>
+  </si>
+  <si>
+    <t>C0008976</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>C1517741</t>
+  </si>
+  <si>
+    <t>30 D (30 Days)</t>
+  </si>
+  <si>
+    <t>C4028326</t>
+  </si>
+  <si>
+    <t>Current (Current (present time))</t>
+  </si>
+  <si>
+    <t>C0521116</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -272,13 +646,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -299,30 +680,86 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -652,347 +1089,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="68.5" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="28">
+      <c r="D1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="28">
+      <c r="D2" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="42">
+      <c r="D10" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="42">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="E11" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="28">
+      <c r="E13" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="28">
+      <c r="E14" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="E15" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="E16" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="28">
+      <c r="E17" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="28">
+      <c r="F18" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28">
+    <row r="20" spans="1:6" ht="28">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="28">
+      <c r="D20" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28">
       <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28">
+    <row r="22" spans="1:6" ht="28">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="28">
+      <c r="D22" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="F23" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="E24" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="28">
+      <c r="D25" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="28">
+      <c r="E26" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28">
       <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28">
+    <row r="28" spans="1:6" ht="28">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="28">
+      <c r="E28" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1008,42 +1508,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="49.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="3" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="34.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9" style="3" customWidth="1"/>
+    <col min="9" max="9" width="14" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="E1" s="7"/>
+      <c r="F1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="1">
@@ -1052,13 +1567,24 @@
       <c r="D2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1067,13 +1593,24 @@
       <c r="D3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1082,13 +1619,24 @@
       <c r="D4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1097,13 +1645,24 @@
       <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1112,13 +1671,24 @@
       <c r="D6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1127,13 +1697,24 @@
       <c r="D7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1142,13 +1723,24 @@
       <c r="D8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1157,12 +1749,24 @@
       <c r="D9" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="1">
@@ -1171,12 +1775,24 @@
       <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="42">
+      <c r="F10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1">
@@ -1185,12 +1801,24 @@
       <c r="D11" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1199,12 +1827,24 @@
       <c r="D12" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C13" s="1">
@@ -1213,12 +1853,24 @@
       <c r="D13" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="28">
+      <c r="F13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="1">
@@ -1227,12 +1879,24 @@
       <c r="D14" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="28">
+      <c r="F14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="1">
@@ -1241,12 +1905,24 @@
       <c r="D15" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="F15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="1">
@@ -1255,12 +1931,24 @@
       <c r="D16" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="F16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="1">
@@ -1269,26 +1957,50 @@
       <c r="D17" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
+      <c r="F17" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="28">
+      <c r="A18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="9">
         <v>75865</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="F18" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1297,12 +2009,24 @@
       <c r="D19" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="F19" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="1">
@@ -1311,12 +2035,24 @@
       <c r="D20" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="F20" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1325,12 +2061,24 @@
       <c r="D21" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="28">
+      <c r="F21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="28">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="1">
@@ -1339,12 +2087,24 @@
       <c r="D22" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="28">
+      <c r="F22" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="28">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="1">
@@ -1353,12 +2113,24 @@
       <c r="D23" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="F23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="1">
@@ -1367,12 +2139,24 @@
       <c r="D24" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="F24" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="1">
@@ -1381,12 +2165,24 @@
       <c r="D25" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="F25" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="1">
@@ -1395,12 +2191,24 @@
       <c r="D26" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="28">
+      <c r="F26" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="28">
       <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1409,12 +2217,24 @@
       <c r="D27" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="F27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="28">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="1">
@@ -1423,12 +2243,24 @@
       <c r="D28" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="28">
+      <c r="F28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="28">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1437,12 +2269,24 @@
       <c r="D29" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="F29" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="28">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="1">
@@ -1451,9 +2295,302 @@
       <c r="D30" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="F30" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="F31" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="F32" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9">
+      <c r="F33" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="6:9">
+      <c r="F34" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9">
+      <c r="F35" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="6:9">
+      <c r="F36" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="6:9">
+      <c r="F37" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="6:9">
+      <c r="F38" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="6:9">
+      <c r="F39" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="6:9">
+      <c r="F40" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="6:9">
+      <c r="F41" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="6:9">
+      <c r="F42" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="6:9">
+      <c r="F43" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="6:9">
+      <c r="F44" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="6:9">
+      <c r="F45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="6:9">
+      <c r="F46" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="6:9">
+      <c r="F47" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="6:9">
+      <c r="F48" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="6:9">
+      <c r="F49" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="6:9">
+      <c r="F50" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>